<commit_message>
move dependencies to requirements_dev.txt
</commit_message>
<xml_diff>
--- a/input/DOI_Reserved_GEO_200318_with_corrected_identifier.xlsx
+++ b/input/DOI_Reserved_GEO_200318_with_corrected_identifier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loubrieu/PycharmProjects/pds-doi-service/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15A20DE-81EC-3546-8631-9959738C30EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F54EF3-EB44-7140-809E-240225C04D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="my_sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>status</t>
   </si>
@@ -43,9 +43,6 @@
     <t>related_resource</t>
   </si>
   <si>
-    <t>submitter_email</t>
-  </si>
-  <si>
     <t>Reserved</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
   </si>
   <si>
     <t>urn:nasa:pds:lab_shocked_feldspars::1.0</t>
-  </si>
-  <si>
-    <t>Bill.Green@my_node</t>
   </si>
   <si>
     <t>Laboratory Shocked Feldspars Collection</t>
@@ -453,7 +447,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H1" sqref="H1:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -485,87 +479,79 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2">
         <v>43901</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="2">
         <v>43902</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="2">
         <v>43902</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="H4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change read engine for xls files
update readme with missing instruction for dev deployement
</commit_message>
<xml_diff>
--- a/input/DOI_Reserved_GEO_200318_with_corrected_identifier.xlsx
+++ b/input/DOI_Reserved_GEO_200318_with_corrected_identifier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loubrieu/PycharmProjects/pds-doi-service/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F54EF3-EB44-7140-809E-240225C04D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E419522-D5FA-774C-9061-7918AE10FC5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="my_sheet" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>J. R.</t>
   </si>
   <si>
-    <t>urn:nasa:pds:lab_shocked_feldspars::1.0</t>
-  </si>
-  <si>
     <t>Laboratory Shocked Feldspars Collection</t>
   </si>
   <si>
@@ -73,16 +70,19 @@
     <t>J2. R2.</t>
   </si>
   <si>
-    <t>urn:nasa:pds:lab_shocked_feldspars_2::1.0</t>
-  </si>
-  <si>
     <t>Johnson_3</t>
   </si>
   <si>
     <t>J3. R3.</t>
   </si>
   <si>
-    <t>urn:nasa:pds:lab_shocked_feldspars_3::1.0</t>
+    <t>urn:nasa:pds:lab_shocked_feldspars::11.0</t>
+  </si>
+  <si>
+    <t>urn:nasa:pds:lab_shocked_feldspars_21::1.0</t>
+  </si>
+  <si>
+    <t>urn:nasa:pds:lab_shocked_feldspars_31::1.0</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2">
         <v>43901</v>
@@ -501,7 +501,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -516,16 +516,16 @@
         <v>43902</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -540,13 +540,13 @@
         <v>43902</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
update README for startup command and service test
</commit_message>
<xml_diff>
--- a/input/DOI_Reserved_GEO_200318_with_corrected_identifier.xlsx
+++ b/input/DOI_Reserved_GEO_200318_with_corrected_identifier.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loubrieu/PycharmProjects/pds-doi-service/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E419522-D5FA-774C-9061-7918AE10FC5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA97419F-6603-F34F-B4B7-9E550D0DCACD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="my_sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -447,7 +447,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Production Server Integration (#166)
* Code cleanup for core/util/config_parser.py and general_util.py

* Code cleanup of the pds_doi_service.core.db package

* Added logging statements to api/controllers/doi_controller.py

* Added waitress to requirements.txt

* Added config entries for api_host and api_port to conf.ini.default

* Integrated use of the waitress application server to the main function of the DOI service API

* Updated name of DOI API to pds-doi-api (from pds_doi_api) in project setup.py

* Fixed typo in pull_request_template.md

* Added openapi-schema-validator and wheel to requirements.txt to satisfy Roundup env

* update README for startup command and service test

Co-authored-by: Scott Collins <collinss@jpl.nasa.gov>
Co-authored-by: thomas loubrieu <thomas.loubrieu@jpl.nasa.gov>
</commit_message>
<xml_diff>
--- a/input/DOI_Reserved_GEO_200318_with_corrected_identifier.xlsx
+++ b/input/DOI_Reserved_GEO_200318_with_corrected_identifier.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loubrieu/PycharmProjects/pds-doi-service/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E419522-D5FA-774C-9061-7918AE10FC5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA97419F-6603-F34F-B4B7-9E550D0DCACD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="my_sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -447,7 +447,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>